<commit_message>
test: update sample datas
</commit_message>
<xml_diff>
--- a/tests/test_comment.xlsx
+++ b/tests/test_comment.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>user_name</t>
+    <t>user</t>
   </si>
   <si>
     <t>article_url</t>
@@ -25,7 +25,7 @@
     <t>content</t>
   </si>
   <si>
-    <t>publication_date</t>
+    <t>comment_date</t>
   </si>
   <si>
     <t>aUko</t>

</xml_diff>